<commit_message>
feat: replace tokens in excel
</commit_message>
<xml_diff>
--- a/tests/Pkup.Console.Tests/pkup_template_sample.xlsx
+++ b/tests/Pkup.Console.Tests/pkup_template_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25917"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\pkup\PKUP\tests\Pkup.Console.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9877AA6D-D838-4FAC-BF31-FB1E9FB6CF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{9877AA6D-D838-4FAC-BF31-FB1E9FB6CF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFA3B8BA-6F7A-4601-93AB-80CFDC2604F7}"/>
   <bookViews>
     <workbookView xWindow="924" yWindow="2388" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,45 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t xml:space="preserve">…………………….. </t>
+      <t xml:space="preserve">{Name} </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>(Employee’s name and last name)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">{JobPosition} </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>(Employee’s job position)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">{StartDate} - {EndDate} </t>
     </r>
     <r>
       <rPr>
@@ -64,34 +102,6 @@
   </si>
   <si>
     <t>Creative works details - description (to be completed by the Employee)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">…………………….. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>(Employee’s job position)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">…………………….. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>(Employee’s name and last name)</t>
-    </r>
   </si>
   <si>
     <t>Who approves (to be completed by Company)</t>
@@ -514,24 +524,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -721,6 +731,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -730,13 +747,6 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -859,7 +869,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A6D021A-DBD4-4D09-9BA0-27D5B25C95BD}" name="Таблица1" displayName="Таблица1" ref="A6:E16" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A6D021A-DBD4-4D09-9BA0-27D5B25C95BD}" name="Таблица1" displayName="Таблица1" ref="A6:E16" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
   <autoFilter ref="A6:E16" xr:uid="{6A6D021A-DBD4-4D09-9BA0-27D5B25C95BD}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{AD913201-42A5-4907-868C-973F8483A5B3}" name="Number" dataDxfId="4"/>
@@ -1953,55 +1963,55 @@
   <dimension ref="A1:E298"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="9.6"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="9.6"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="9.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="38.25" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" ht="28.35" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-    </row>
-    <row r="3" spans="1:5" ht="28.35" customHeight="1">
-      <c r="A3" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-    </row>
-    <row r="4" spans="1:5" ht="28.35" customHeight="1">
-      <c r="A4" s="37" t="s">
+      <c r="B2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="31"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="36"/>
+    </row>
+    <row r="3" spans="1:5" ht="28.35" customHeight="1">
+      <c r="A3" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
+    </row>
+    <row r="4" spans="1:5" ht="28.35" customHeight="1">
+      <c r="A4" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5" ht="8.1" customHeight="1">
       <c r="A5" s="5"/>
@@ -2012,13 +2022,13 @@
     </row>
     <row r="6" spans="1:5" ht="33" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>7</v>
@@ -2117,12 +2127,12 @@
       <c r="D16" s="28"/>
       <c r="E16" s="29"/>
     </row>
-    <row r="17" spans="1:5" ht="13.65" customHeight="1">
+    <row r="17" spans="1:5" ht="13.7" customHeight="1">
       <c r="A17" s="14"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="33"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
     </row>
     <row r="18" spans="1:5" ht="9.75" customHeight="1">
       <c r="A18" s="2"/>
@@ -2145,12 +2155,12 @@
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="13.65" customHeight="1">
+    <row r="21" spans="1:5" ht="13.7" customHeight="1">
       <c r="A21" s="2"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="31"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="36"/>
     </row>
     <row r="22" spans="1:5" ht="9.75" customHeight="1">
       <c r="A22" s="2"/>
@@ -2194,12 +2204,12 @@
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" ht="13.65" customHeight="1">
+    <row r="28" spans="1:5" ht="13.7" customHeight="1">
       <c r="A28" s="2"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="36"/>
     </row>
     <row r="29" spans="1:5" ht="9.75" customHeight="1">
       <c r="A29" s="2"/>
@@ -2243,12 +2253,12 @@
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" ht="13.65" customHeight="1">
+    <row r="35" spans="1:5" ht="13.7" customHeight="1">
       <c r="A35" s="2"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="31"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="36"/>
     </row>
     <row r="36" spans="1:5" ht="9.75" customHeight="1">
       <c r="A36" s="2"/>
@@ -2271,12 +2281,12 @@
       <c r="D38" s="3"/>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:5" ht="13.65" customHeight="1">
+    <row r="39" spans="1:5" ht="13.7" customHeight="1">
       <c r="A39" s="2"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="31"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="36"/>
     </row>
     <row r="40" spans="1:5" ht="9.75" customHeight="1">
       <c r="A40" s="2"/>
@@ -2299,12 +2309,12 @@
       <c r="D42" s="3"/>
       <c r="E42" s="4"/>
     </row>
-    <row r="43" spans="1:5" ht="13.65" customHeight="1">
+    <row r="43" spans="1:5" ht="13.7" customHeight="1">
       <c r="A43" s="2"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="31"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="36"/>
     </row>
     <row r="44" spans="1:5" ht="9.75" customHeight="1">
       <c r="A44" s="2"/>
@@ -2327,12 +2337,12 @@
       <c r="D46" s="3"/>
       <c r="E46" s="4"/>
     </row>
-    <row r="47" spans="1:5" ht="13.65" customHeight="1">
+    <row r="47" spans="1:5" ht="13.7" customHeight="1">
       <c r="A47" s="2"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="31"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="36"/>
     </row>
     <row r="48" spans="1:5" ht="9.75" customHeight="1">
       <c r="A48" s="2"/>
@@ -2376,12 +2386,12 @@
       <c r="D53" s="3"/>
       <c r="E53" s="4"/>
     </row>
-    <row r="54" spans="1:5" ht="13.65" customHeight="1">
+    <row r="54" spans="1:5" ht="13.7" customHeight="1">
       <c r="A54" s="2"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="31"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="36"/>
     </row>
     <row r="55" spans="1:5" ht="9.75" customHeight="1">
       <c r="A55" s="2"/>
@@ -2404,12 +2414,12 @@
       <c r="D57" s="3"/>
       <c r="E57" s="4"/>
     </row>
-    <row r="58" spans="1:5" ht="13.65" customHeight="1">
+    <row r="58" spans="1:5" ht="13.7" customHeight="1">
       <c r="A58" s="2"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="31"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="36"/>
     </row>
     <row r="59" spans="1:5" ht="9.75" customHeight="1">
       <c r="A59" s="2"/>
@@ -2432,12 +2442,12 @@
       <c r="D61" s="3"/>
       <c r="E61" s="4"/>
     </row>
-    <row r="62" spans="1:5" ht="13.65" customHeight="1">
+    <row r="62" spans="1:5" ht="13.7" customHeight="1">
       <c r="A62" s="2"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="31"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="36"/>
     </row>
     <row r="63" spans="1:5" ht="9.75" customHeight="1">
       <c r="A63" s="2"/>
@@ -2460,12 +2470,12 @@
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
     </row>
-    <row r="66" spans="1:5" ht="13.65" customHeight="1">
+    <row r="66" spans="1:5" ht="13.7" customHeight="1">
       <c r="A66" s="2"/>
-      <c r="B66" s="30"/>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="31"/>
+      <c r="B66" s="35"/>
+      <c r="C66" s="35"/>
+      <c r="D66" s="35"/>
+      <c r="E66" s="36"/>
     </row>
     <row r="67" spans="1:5" ht="9.75" customHeight="1">
       <c r="A67" s="2"/>
@@ -2551,12 +2561,12 @@
       <c r="D78" s="3"/>
       <c r="E78" s="4"/>
     </row>
-    <row r="79" spans="1:5" ht="13.65" customHeight="1">
+    <row r="79" spans="1:5" ht="13.7" customHeight="1">
       <c r="A79" s="2"/>
-      <c r="B79" s="30"/>
-      <c r="C79" s="30"/>
-      <c r="D79" s="30"/>
-      <c r="E79" s="31"/>
+      <c r="B79" s="35"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="35"/>
+      <c r="E79" s="36"/>
     </row>
     <row r="80" spans="1:5" ht="9.75" customHeight="1">
       <c r="A80" s="2"/>
@@ -2579,12 +2589,12 @@
       <c r="D82" s="3"/>
       <c r="E82" s="4"/>
     </row>
-    <row r="83" spans="1:5" ht="13.65" customHeight="1">
+    <row r="83" spans="1:5" ht="13.7" customHeight="1">
       <c r="A83" s="2"/>
-      <c r="B83" s="30"/>
-      <c r="C83" s="30"/>
-      <c r="D83" s="30"/>
-      <c r="E83" s="31"/>
+      <c r="B83" s="35"/>
+      <c r="C83" s="35"/>
+      <c r="D83" s="35"/>
+      <c r="E83" s="36"/>
     </row>
     <row r="84" spans="1:5" ht="9.75" customHeight="1">
       <c r="A84" s="2"/>
@@ -2691,12 +2701,12 @@
       <c r="D98" s="3"/>
       <c r="E98" s="4"/>
     </row>
-    <row r="99" spans="1:5" ht="13.65" customHeight="1">
+    <row r="99" spans="1:5" ht="13.7" customHeight="1">
       <c r="A99" s="2"/>
-      <c r="B99" s="30"/>
-      <c r="C99" s="30"/>
-      <c r="D99" s="30"/>
-      <c r="E99" s="31"/>
+      <c r="B99" s="35"/>
+      <c r="C99" s="35"/>
+      <c r="D99" s="35"/>
+      <c r="E99" s="36"/>
     </row>
     <row r="100" spans="1:5" ht="9.75" customHeight="1">
       <c r="A100" s="2"/>
@@ -2719,12 +2729,12 @@
       <c r="D102" s="3"/>
       <c r="E102" s="4"/>
     </row>
-    <row r="103" spans="1:5" ht="13.65" customHeight="1">
+    <row r="103" spans="1:5" ht="13.7" customHeight="1">
       <c r="A103" s="2"/>
-      <c r="B103" s="30"/>
-      <c r="C103" s="30"/>
-      <c r="D103" s="30"/>
-      <c r="E103" s="31"/>
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="35"/>
+      <c r="E103" s="36"/>
     </row>
     <row r="104" spans="1:5" ht="9.75" customHeight="1">
       <c r="A104" s="2"/>
@@ -2747,12 +2757,12 @@
       <c r="D106" s="3"/>
       <c r="E106" s="4"/>
     </row>
-    <row r="107" spans="1:5" ht="13.65" customHeight="1">
+    <row r="107" spans="1:5" ht="13.7" customHeight="1">
       <c r="A107" s="2"/>
-      <c r="B107" s="30"/>
-      <c r="C107" s="30"/>
-      <c r="D107" s="30"/>
-      <c r="E107" s="31"/>
+      <c r="B107" s="35"/>
+      <c r="C107" s="35"/>
+      <c r="D107" s="35"/>
+      <c r="E107" s="36"/>
     </row>
     <row r="108" spans="1:5" ht="9.75" customHeight="1">
       <c r="A108" s="2"/>
@@ -2796,12 +2806,12 @@
       <c r="D113" s="3"/>
       <c r="E113" s="4"/>
     </row>
-    <row r="114" spans="1:5" ht="13.65" customHeight="1">
+    <row r="114" spans="1:5" ht="13.7" customHeight="1">
       <c r="A114" s="2"/>
-      <c r="B114" s="30"/>
-      <c r="C114" s="30"/>
-      <c r="D114" s="30"/>
-      <c r="E114" s="31"/>
+      <c r="B114" s="35"/>
+      <c r="C114" s="35"/>
+      <c r="D114" s="35"/>
+      <c r="E114" s="36"/>
     </row>
     <row r="115" spans="1:5" ht="9.75" customHeight="1">
       <c r="A115" s="2"/>
@@ -2824,12 +2834,12 @@
       <c r="D117" s="3"/>
       <c r="E117" s="4"/>
     </row>
-    <row r="118" spans="1:5" ht="13.65" customHeight="1">
+    <row r="118" spans="1:5" ht="13.7" customHeight="1">
       <c r="A118" s="2"/>
-      <c r="B118" s="30"/>
-      <c r="C118" s="30"/>
-      <c r="D118" s="30"/>
-      <c r="E118" s="31"/>
+      <c r="B118" s="35"/>
+      <c r="C118" s="35"/>
+      <c r="D118" s="35"/>
+      <c r="E118" s="36"/>
     </row>
     <row r="119" spans="1:5" ht="9.75" customHeight="1">
       <c r="A119" s="2"/>
@@ -2852,12 +2862,12 @@
       <c r="D121" s="3"/>
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="1:5" ht="13.65" customHeight="1">
+    <row r="122" spans="1:5" ht="13.7" customHeight="1">
       <c r="A122" s="2"/>
-      <c r="B122" s="30"/>
-      <c r="C122" s="30"/>
-      <c r="D122" s="30"/>
-      <c r="E122" s="31"/>
+      <c r="B122" s="35"/>
+      <c r="C122" s="35"/>
+      <c r="D122" s="35"/>
+      <c r="E122" s="36"/>
     </row>
     <row r="123" spans="1:5" ht="9.75" customHeight="1">
       <c r="A123" s="2"/>
@@ -2880,12 +2890,12 @@
       <c r="D125" s="3"/>
       <c r="E125" s="4"/>
     </row>
-    <row r="126" spans="1:5" ht="13.65" customHeight="1">
+    <row r="126" spans="1:5" ht="13.7" customHeight="1">
       <c r="A126" s="2"/>
-      <c r="B126" s="30"/>
-      <c r="C126" s="30"/>
-      <c r="D126" s="30"/>
-      <c r="E126" s="31"/>
+      <c r="B126" s="35"/>
+      <c r="C126" s="35"/>
+      <c r="D126" s="35"/>
+      <c r="E126" s="36"/>
     </row>
     <row r="127" spans="1:5" ht="9.75" customHeight="1">
       <c r="A127" s="2"/>
@@ -2929,12 +2939,12 @@
       <c r="D132" s="3"/>
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="1:5" ht="13.65" customHeight="1">
+    <row r="133" spans="1:5" ht="13.7" customHeight="1">
       <c r="A133" s="2"/>
-      <c r="B133" s="30"/>
-      <c r="C133" s="30"/>
-      <c r="D133" s="30"/>
-      <c r="E133" s="31"/>
+      <c r="B133" s="35"/>
+      <c r="C133" s="35"/>
+      <c r="D133" s="35"/>
+      <c r="E133" s="36"/>
     </row>
     <row r="134" spans="1:5" ht="9.75" customHeight="1">
       <c r="A134" s="2"/>
@@ -2957,12 +2967,12 @@
       <c r="D136" s="3"/>
       <c r="E136" s="4"/>
     </row>
-    <row r="137" spans="1:5" ht="13.65" customHeight="1">
+    <row r="137" spans="1:5" ht="13.7" customHeight="1">
       <c r="A137" s="2"/>
-      <c r="B137" s="30"/>
-      <c r="C137" s="30"/>
-      <c r="D137" s="30"/>
-      <c r="E137" s="31"/>
+      <c r="B137" s="35"/>
+      <c r="C137" s="35"/>
+      <c r="D137" s="35"/>
+      <c r="E137" s="36"/>
     </row>
     <row r="138" spans="1:5" ht="9.75" customHeight="1">
       <c r="A138" s="2"/>
@@ -2985,12 +2995,12 @@
       <c r="D140" s="3"/>
       <c r="E140" s="4"/>
     </row>
-    <row r="141" spans="1:5" ht="13.65" customHeight="1">
+    <row r="141" spans="1:5" ht="13.7" customHeight="1">
       <c r="A141" s="2"/>
-      <c r="B141" s="30"/>
-      <c r="C141" s="30"/>
-      <c r="D141" s="30"/>
-      <c r="E141" s="31"/>
+      <c r="B141" s="35"/>
+      <c r="C141" s="35"/>
+      <c r="D141" s="35"/>
+      <c r="E141" s="36"/>
     </row>
     <row r="142" spans="1:5" ht="9.75" customHeight="1">
       <c r="A142" s="2"/>
@@ -3013,12 +3023,12 @@
       <c r="D144" s="3"/>
       <c r="E144" s="4"/>
     </row>
-    <row r="145" spans="1:5" ht="13.65" customHeight="1">
+    <row r="145" spans="1:5" ht="13.7" customHeight="1">
       <c r="A145" s="2"/>
-      <c r="B145" s="30"/>
-      <c r="C145" s="30"/>
-      <c r="D145" s="30"/>
-      <c r="E145" s="31"/>
+      <c r="B145" s="35"/>
+      <c r="C145" s="35"/>
+      <c r="D145" s="35"/>
+      <c r="E145" s="36"/>
     </row>
     <row r="146" spans="1:5" ht="9.75" customHeight="1">
       <c r="A146" s="2"/>
@@ -3041,12 +3051,12 @@
       <c r="D148" s="3"/>
       <c r="E148" s="4"/>
     </row>
-    <row r="149" spans="1:5" ht="13.65" customHeight="1">
+    <row r="149" spans="1:5" ht="13.7" customHeight="1">
       <c r="A149" s="2"/>
-      <c r="B149" s="30"/>
-      <c r="C149" s="30"/>
-      <c r="D149" s="30"/>
-      <c r="E149" s="31"/>
+      <c r="B149" s="35"/>
+      <c r="C149" s="35"/>
+      <c r="D149" s="35"/>
+      <c r="E149" s="36"/>
     </row>
     <row r="150" spans="1:5" ht="9.75" customHeight="1">
       <c r="A150" s="2"/>
@@ -3069,12 +3079,12 @@
       <c r="D152" s="3"/>
       <c r="E152" s="4"/>
     </row>
-    <row r="153" spans="1:5" ht="13.65" customHeight="1">
+    <row r="153" spans="1:5" ht="13.7" customHeight="1">
       <c r="A153" s="2"/>
-      <c r="B153" s="30"/>
-      <c r="C153" s="30"/>
-      <c r="D153" s="30"/>
-      <c r="E153" s="31"/>
+      <c r="B153" s="35"/>
+      <c r="C153" s="35"/>
+      <c r="D153" s="35"/>
+      <c r="E153" s="36"/>
     </row>
     <row r="154" spans="1:5" ht="9.75" customHeight="1">
       <c r="A154" s="2"/>
@@ -3097,12 +3107,12 @@
       <c r="D156" s="3"/>
       <c r="E156" s="4"/>
     </row>
-    <row r="157" spans="1:5" ht="13.65" customHeight="1">
+    <row r="157" spans="1:5" ht="13.7" customHeight="1">
       <c r="A157" s="2"/>
-      <c r="B157" s="30"/>
-      <c r="C157" s="30"/>
-      <c r="D157" s="30"/>
-      <c r="E157" s="31"/>
+      <c r="B157" s="35"/>
+      <c r="C157" s="35"/>
+      <c r="D157" s="35"/>
+      <c r="E157" s="36"/>
     </row>
     <row r="158" spans="1:5" ht="9.75" customHeight="1">
       <c r="A158" s="2"/>
@@ -3125,12 +3135,12 @@
       <c r="D160" s="3"/>
       <c r="E160" s="4"/>
     </row>
-    <row r="161" spans="1:5" ht="13.65" customHeight="1">
+    <row r="161" spans="1:5" ht="13.7" customHeight="1">
       <c r="A161" s="2"/>
-      <c r="B161" s="30"/>
-      <c r="C161" s="30"/>
-      <c r="D161" s="30"/>
-      <c r="E161" s="31"/>
+      <c r="B161" s="35"/>
+      <c r="C161" s="35"/>
+      <c r="D161" s="35"/>
+      <c r="E161" s="36"/>
     </row>
     <row r="162" spans="1:5" ht="9.75" customHeight="1">
       <c r="A162" s="2"/>
@@ -3216,12 +3226,12 @@
       <c r="D173" s="3"/>
       <c r="E173" s="4"/>
     </row>
-    <row r="174" spans="1:5" ht="13.65" customHeight="1">
+    <row r="174" spans="1:5" ht="13.7" customHeight="1">
       <c r="A174" s="2"/>
-      <c r="B174" s="30"/>
-      <c r="C174" s="30"/>
-      <c r="D174" s="30"/>
-      <c r="E174" s="31"/>
+      <c r="B174" s="35"/>
+      <c r="C174" s="35"/>
+      <c r="D174" s="35"/>
+      <c r="E174" s="36"/>
     </row>
     <row r="175" spans="1:5" ht="9.75" customHeight="1">
       <c r="A175" s="2"/>
@@ -3265,12 +3275,12 @@
       <c r="D180" s="3"/>
       <c r="E180" s="4"/>
     </row>
-    <row r="181" spans="1:5" ht="13.65" customHeight="1">
+    <row r="181" spans="1:5" ht="13.7" customHeight="1">
       <c r="A181" s="2"/>
-      <c r="B181" s="30"/>
-      <c r="C181" s="30"/>
-      <c r="D181" s="30"/>
-      <c r="E181" s="31"/>
+      <c r="B181" s="35"/>
+      <c r="C181" s="35"/>
+      <c r="D181" s="35"/>
+      <c r="E181" s="36"/>
     </row>
     <row r="182" spans="1:5" ht="9.75" customHeight="1">
       <c r="A182" s="2"/>
@@ -3314,12 +3324,12 @@
       <c r="D187" s="3"/>
       <c r="E187" s="4"/>
     </row>
-    <row r="188" spans="1:5" ht="13.65" customHeight="1">
+    <row r="188" spans="1:5" ht="13.7" customHeight="1">
       <c r="A188" s="2"/>
-      <c r="B188" s="30"/>
-      <c r="C188" s="30"/>
-      <c r="D188" s="30"/>
-      <c r="E188" s="31"/>
+      <c r="B188" s="35"/>
+      <c r="C188" s="35"/>
+      <c r="D188" s="35"/>
+      <c r="E188" s="36"/>
     </row>
     <row r="189" spans="1:5" ht="9.75" customHeight="1">
       <c r="A189" s="2"/>
@@ -3342,12 +3352,12 @@
       <c r="D191" s="3"/>
       <c r="E191" s="4"/>
     </row>
-    <row r="192" spans="1:5" ht="13.65" customHeight="1">
+    <row r="192" spans="1:5" ht="13.7" customHeight="1">
       <c r="A192" s="2"/>
-      <c r="B192" s="30"/>
-      <c r="C192" s="30"/>
-      <c r="D192" s="30"/>
-      <c r="E192" s="31"/>
+      <c r="B192" s="35"/>
+      <c r="C192" s="35"/>
+      <c r="D192" s="35"/>
+      <c r="E192" s="36"/>
     </row>
     <row r="193" spans="1:5" ht="9.75" customHeight="1">
       <c r="A193" s="2"/>
@@ -3391,12 +3401,12 @@
       <c r="D198" s="3"/>
       <c r="E198" s="4"/>
     </row>
-    <row r="199" spans="1:5" ht="13.65" customHeight="1">
+    <row r="199" spans="1:5" ht="13.7" customHeight="1">
       <c r="A199" s="2"/>
-      <c r="B199" s="30"/>
-      <c r="C199" s="30"/>
-      <c r="D199" s="30"/>
-      <c r="E199" s="31"/>
+      <c r="B199" s="35"/>
+      <c r="C199" s="35"/>
+      <c r="D199" s="35"/>
+      <c r="E199" s="36"/>
     </row>
     <row r="200" spans="1:5" ht="9.75" customHeight="1">
       <c r="A200" s="2"/>
@@ -3419,12 +3429,12 @@
       <c r="D202" s="3"/>
       <c r="E202" s="4"/>
     </row>
-    <row r="203" spans="1:5" ht="13.65" customHeight="1">
+    <row r="203" spans="1:5" ht="13.7" customHeight="1">
       <c r="A203" s="2"/>
-      <c r="B203" s="30"/>
-      <c r="C203" s="30"/>
-      <c r="D203" s="30"/>
-      <c r="E203" s="31"/>
+      <c r="B203" s="35"/>
+      <c r="C203" s="35"/>
+      <c r="D203" s="35"/>
+      <c r="E203" s="36"/>
     </row>
     <row r="204" spans="1:5" ht="9.75" customHeight="1">
       <c r="A204" s="2"/>
@@ -3447,12 +3457,12 @@
       <c r="D206" s="3"/>
       <c r="E206" s="4"/>
     </row>
-    <row r="207" spans="1:5" ht="13.65" customHeight="1">
+    <row r="207" spans="1:5" ht="13.7" customHeight="1">
       <c r="A207" s="2"/>
-      <c r="B207" s="30"/>
-      <c r="C207" s="30"/>
-      <c r="D207" s="30"/>
-      <c r="E207" s="31"/>
+      <c r="B207" s="35"/>
+      <c r="C207" s="35"/>
+      <c r="D207" s="35"/>
+      <c r="E207" s="36"/>
     </row>
     <row r="208" spans="1:5" ht="9.75" customHeight="1">
       <c r="A208" s="2"/>
@@ -3475,12 +3485,12 @@
       <c r="D210" s="3"/>
       <c r="E210" s="4"/>
     </row>
-    <row r="211" spans="1:5" ht="13.65" customHeight="1">
+    <row r="211" spans="1:5" ht="13.7" customHeight="1">
       <c r="A211" s="2"/>
-      <c r="B211" s="30"/>
-      <c r="C211" s="30"/>
-      <c r="D211" s="30"/>
-      <c r="E211" s="31"/>
+      <c r="B211" s="35"/>
+      <c r="C211" s="35"/>
+      <c r="D211" s="35"/>
+      <c r="E211" s="36"/>
     </row>
     <row r="212" spans="1:5" ht="9.75" customHeight="1">
       <c r="A212" s="2"/>
@@ -3503,12 +3513,12 @@
       <c r="D214" s="3"/>
       <c r="E214" s="4"/>
     </row>
-    <row r="215" spans="1:5" ht="13.65" customHeight="1">
+    <row r="215" spans="1:5" ht="13.7" customHeight="1">
       <c r="A215" s="2"/>
-      <c r="B215" s="30"/>
-      <c r="C215" s="30"/>
-      <c r="D215" s="30"/>
-      <c r="E215" s="31"/>
+      <c r="B215" s="35"/>
+      <c r="C215" s="35"/>
+      <c r="D215" s="35"/>
+      <c r="E215" s="36"/>
     </row>
     <row r="216" spans="1:5" ht="9.75" customHeight="1">
       <c r="A216" s="2"/>
@@ -3531,12 +3541,12 @@
       <c r="D218" s="3"/>
       <c r="E218" s="4"/>
     </row>
-    <row r="219" spans="1:5" ht="13.65" customHeight="1">
+    <row r="219" spans="1:5" ht="13.7" customHeight="1">
       <c r="A219" s="2"/>
-      <c r="B219" s="30"/>
-      <c r="C219" s="30"/>
-      <c r="D219" s="30"/>
-      <c r="E219" s="31"/>
+      <c r="B219" s="35"/>
+      <c r="C219" s="35"/>
+      <c r="D219" s="35"/>
+      <c r="E219" s="36"/>
     </row>
     <row r="220" spans="1:5" ht="9.75" customHeight="1">
       <c r="A220" s="2"/>
@@ -3559,12 +3569,12 @@
       <c r="D222" s="3"/>
       <c r="E222" s="4"/>
     </row>
-    <row r="223" spans="1:5" ht="13.65" customHeight="1">
+    <row r="223" spans="1:5" ht="13.7" customHeight="1">
       <c r="A223" s="2"/>
-      <c r="B223" s="30"/>
-      <c r="C223" s="30"/>
-      <c r="D223" s="30"/>
-      <c r="E223" s="31"/>
+      <c r="B223" s="35"/>
+      <c r="C223" s="35"/>
+      <c r="D223" s="35"/>
+      <c r="E223" s="36"/>
     </row>
     <row r="224" spans="1:5" ht="9.75" customHeight="1">
       <c r="A224" s="2"/>
@@ -3587,12 +3597,12 @@
       <c r="D226" s="3"/>
       <c r="E226" s="4"/>
     </row>
-    <row r="227" spans="1:5" ht="13.65" customHeight="1">
+    <row r="227" spans="1:5" ht="13.7" customHeight="1">
       <c r="A227" s="2"/>
-      <c r="B227" s="30"/>
-      <c r="C227" s="30"/>
-      <c r="D227" s="30"/>
-      <c r="E227" s="31"/>
+      <c r="B227" s="35"/>
+      <c r="C227" s="35"/>
+      <c r="D227" s="35"/>
+      <c r="E227" s="36"/>
     </row>
     <row r="228" spans="1:5" ht="9.75" customHeight="1">
       <c r="A228" s="2"/>
@@ -3657,12 +3667,12 @@
       <c r="D236" s="3"/>
       <c r="E236" s="4"/>
     </row>
-    <row r="237" spans="1:5" ht="13.65" customHeight="1">
+    <row r="237" spans="1:5" ht="13.7" customHeight="1">
       <c r="A237" s="2"/>
-      <c r="B237" s="30"/>
-      <c r="C237" s="30"/>
-      <c r="D237" s="30"/>
-      <c r="E237" s="31"/>
+      <c r="B237" s="35"/>
+      <c r="C237" s="35"/>
+      <c r="D237" s="35"/>
+      <c r="E237" s="36"/>
     </row>
     <row r="238" spans="1:5" ht="9.75" customHeight="1">
       <c r="A238" s="2"/>
@@ -3685,12 +3695,12 @@
       <c r="D240" s="3"/>
       <c r="E240" s="4"/>
     </row>
-    <row r="241" spans="1:5" ht="13.65" customHeight="1">
+    <row r="241" spans="1:5" ht="13.7" customHeight="1">
       <c r="A241" s="2"/>
-      <c r="B241" s="30"/>
-      <c r="C241" s="30"/>
-      <c r="D241" s="30"/>
-      <c r="E241" s="31"/>
+      <c r="B241" s="35"/>
+      <c r="C241" s="35"/>
+      <c r="D241" s="35"/>
+      <c r="E241" s="36"/>
     </row>
     <row r="242" spans="1:5" ht="9.75" customHeight="1">
       <c r="A242" s="2"/>
@@ -3713,12 +3723,12 @@
       <c r="D244" s="3"/>
       <c r="E244" s="4"/>
     </row>
-    <row r="245" spans="1:5" ht="13.65" customHeight="1">
+    <row r="245" spans="1:5" ht="13.7" customHeight="1">
       <c r="A245" s="2"/>
-      <c r="B245" s="30"/>
-      <c r="C245" s="30"/>
-      <c r="D245" s="30"/>
-      <c r="E245" s="31"/>
+      <c r="B245" s="35"/>
+      <c r="C245" s="35"/>
+      <c r="D245" s="35"/>
+      <c r="E245" s="36"/>
     </row>
     <row r="246" spans="1:5" ht="9.75" customHeight="1">
       <c r="A246" s="2"/>
@@ -3741,12 +3751,12 @@
       <c r="D248" s="3"/>
       <c r="E248" s="4"/>
     </row>
-    <row r="249" spans="1:5" ht="13.65" customHeight="1">
+    <row r="249" spans="1:5" ht="13.7" customHeight="1">
       <c r="A249" s="2"/>
-      <c r="B249" s="30"/>
-      <c r="C249" s="30"/>
-      <c r="D249" s="30"/>
-      <c r="E249" s="31"/>
+      <c r="B249" s="35"/>
+      <c r="C249" s="35"/>
+      <c r="D249" s="35"/>
+      <c r="E249" s="36"/>
     </row>
     <row r="250" spans="1:5" ht="9.75" customHeight="1">
       <c r="A250" s="2"/>
@@ -3769,12 +3779,12 @@
       <c r="D252" s="3"/>
       <c r="E252" s="4"/>
     </row>
-    <row r="253" spans="1:5" ht="13.65" customHeight="1">
+    <row r="253" spans="1:5" ht="13.7" customHeight="1">
       <c r="A253" s="2"/>
-      <c r="B253" s="30"/>
-      <c r="C253" s="30"/>
-      <c r="D253" s="30"/>
-      <c r="E253" s="31"/>
+      <c r="B253" s="35"/>
+      <c r="C253" s="35"/>
+      <c r="D253" s="35"/>
+      <c r="E253" s="36"/>
     </row>
     <row r="254" spans="1:5" ht="9.75" customHeight="1">
       <c r="A254" s="2"/>
@@ -3797,12 +3807,12 @@
       <c r="D256" s="3"/>
       <c r="E256" s="4"/>
     </row>
-    <row r="257" spans="1:5" ht="13.65" customHeight="1">
+    <row r="257" spans="1:5" ht="13.7" customHeight="1">
       <c r="A257" s="2"/>
-      <c r="B257" s="30"/>
-      <c r="C257" s="30"/>
-      <c r="D257" s="30"/>
-      <c r="E257" s="31"/>
+      <c r="B257" s="35"/>
+      <c r="C257" s="35"/>
+      <c r="D257" s="35"/>
+      <c r="E257" s="36"/>
     </row>
     <row r="258" spans="1:5" ht="9.75" customHeight="1">
       <c r="A258" s="2"/>
@@ -3825,12 +3835,12 @@
       <c r="D260" s="3"/>
       <c r="E260" s="4"/>
     </row>
-    <row r="261" spans="1:5" ht="13.65" customHeight="1">
+    <row r="261" spans="1:5" ht="13.7" customHeight="1">
       <c r="A261" s="2"/>
-      <c r="B261" s="30"/>
-      <c r="C261" s="30"/>
-      <c r="D261" s="30"/>
-      <c r="E261" s="31"/>
+      <c r="B261" s="35"/>
+      <c r="C261" s="35"/>
+      <c r="D261" s="35"/>
+      <c r="E261" s="36"/>
     </row>
     <row r="262" spans="1:5" ht="9.75" customHeight="1">
       <c r="A262" s="2"/>
@@ -3979,12 +3989,12 @@
       <c r="D282" s="3"/>
       <c r="E282" s="4"/>
     </row>
-    <row r="283" spans="1:5" ht="13.65" customHeight="1">
+    <row r="283" spans="1:5" ht="13.7" customHeight="1">
       <c r="A283" s="2"/>
-      <c r="B283" s="30"/>
-      <c r="C283" s="30"/>
-      <c r="D283" s="30"/>
-      <c r="E283" s="31"/>
+      <c r="B283" s="35"/>
+      <c r="C283" s="35"/>
+      <c r="D283" s="35"/>
+      <c r="E283" s="36"/>
     </row>
     <row r="284" spans="1:5" ht="9.75" customHeight="1">
       <c r="A284" s="2"/>
@@ -4028,12 +4038,12 @@
       <c r="D289" s="3"/>
       <c r="E289" s="4"/>
     </row>
-    <row r="290" spans="1:5" ht="13.65" customHeight="1">
+    <row r="290" spans="1:5" ht="13.7" customHeight="1">
       <c r="A290" s="2"/>
-      <c r="B290" s="30"/>
-      <c r="C290" s="30"/>
-      <c r="D290" s="30"/>
-      <c r="E290" s="31"/>
+      <c r="B290" s="35"/>
+      <c r="C290" s="35"/>
+      <c r="D290" s="35"/>
+      <c r="E290" s="36"/>
     </row>
     <row r="291" spans="1:5" ht="9.75" customHeight="1">
       <c r="A291" s="2"/>
@@ -4077,12 +4087,12 @@
       <c r="D296" s="3"/>
       <c r="E296" s="4"/>
     </row>
-    <row r="297" spans="1:5" ht="13.65" customHeight="1">
+    <row r="297" spans="1:5" ht="13.7" customHeight="1">
       <c r="A297" s="2"/>
-      <c r="B297" s="30"/>
-      <c r="C297" s="30"/>
-      <c r="D297" s="30"/>
-      <c r="E297" s="31"/>
+      <c r="B297" s="35"/>
+      <c r="C297" s="35"/>
+      <c r="D297" s="35"/>
+      <c r="E297" s="36"/>
     </row>
     <row r="298" spans="1:5" ht="9.6" customHeight="1">
       <c r="A298" s="15"/>
@@ -4093,53 +4103,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B297:E297"/>
-    <mergeCell ref="B290:E290"/>
-    <mergeCell ref="B283:E283"/>
-    <mergeCell ref="B257:E257"/>
-    <mergeCell ref="B261:E261"/>
-    <mergeCell ref="B253:E253"/>
-    <mergeCell ref="B245:E245"/>
-    <mergeCell ref="B249:E249"/>
-    <mergeCell ref="B241:E241"/>
-    <mergeCell ref="B237:E237"/>
-    <mergeCell ref="B227:E227"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="B215:E215"/>
-    <mergeCell ref="B219:E219"/>
-    <mergeCell ref="B211:E211"/>
-    <mergeCell ref="B203:E203"/>
-    <mergeCell ref="B207:E207"/>
-    <mergeCell ref="B199:E199"/>
-    <mergeCell ref="B192:E192"/>
-    <mergeCell ref="B188:E188"/>
-    <mergeCell ref="B181:E181"/>
-    <mergeCell ref="B174:E174"/>
-    <mergeCell ref="B161:E161"/>
-    <mergeCell ref="B157:E157"/>
-    <mergeCell ref="B149:E149"/>
-    <mergeCell ref="B153:E153"/>
-    <mergeCell ref="B145:E145"/>
-    <mergeCell ref="B137:E137"/>
-    <mergeCell ref="B141:E141"/>
-    <mergeCell ref="B133:E133"/>
-    <mergeCell ref="B126:E126"/>
-    <mergeCell ref="B118:E118"/>
-    <mergeCell ref="B122:E122"/>
-    <mergeCell ref="B114:E114"/>
-    <mergeCell ref="B107:E107"/>
-    <mergeCell ref="B103:E103"/>
-    <mergeCell ref="B99:E99"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B39:E39"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B21:E21"/>
@@ -4147,6 +4110,53 @@
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A3:E3"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B99:E99"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B118:E118"/>
+    <mergeCell ref="B122:E122"/>
+    <mergeCell ref="B114:E114"/>
+    <mergeCell ref="B107:E107"/>
+    <mergeCell ref="B103:E103"/>
+    <mergeCell ref="B145:E145"/>
+    <mergeCell ref="B137:E137"/>
+    <mergeCell ref="B141:E141"/>
+    <mergeCell ref="B133:E133"/>
+    <mergeCell ref="B126:E126"/>
+    <mergeCell ref="B181:E181"/>
+    <mergeCell ref="B174:E174"/>
+    <mergeCell ref="B161:E161"/>
+    <mergeCell ref="B157:E157"/>
+    <mergeCell ref="B149:E149"/>
+    <mergeCell ref="B153:E153"/>
+    <mergeCell ref="B203:E203"/>
+    <mergeCell ref="B207:E207"/>
+    <mergeCell ref="B199:E199"/>
+    <mergeCell ref="B192:E192"/>
+    <mergeCell ref="B188:E188"/>
+    <mergeCell ref="B227:E227"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="B215:E215"/>
+    <mergeCell ref="B219:E219"/>
+    <mergeCell ref="B211:E211"/>
+    <mergeCell ref="B253:E253"/>
+    <mergeCell ref="B245:E245"/>
+    <mergeCell ref="B249:E249"/>
+    <mergeCell ref="B241:E241"/>
+    <mergeCell ref="B237:E237"/>
+    <mergeCell ref="B297:E297"/>
+    <mergeCell ref="B290:E290"/>
+    <mergeCell ref="B283:E283"/>
+    <mergeCell ref="B257:E257"/>
+    <mergeCell ref="B261:E261"/>
   </mergeCells>
   <pageMargins left="0.19685" right="0" top="0.19685" bottom="0.49212600000000001" header="0.19685" footer="0.19685"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
feat: add posibility to specify date format
</commit_message>
<xml_diff>
--- a/tests/Pkup.Console.Tests/pkup_template_sample.xlsx
+++ b/tests/Pkup.Console.Tests/pkup_template_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\pkup\PKUP\tests\Pkup.Console.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{9877AA6D-D838-4FAC-BF31-FB1E9FB6CF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFA3B8BA-6F7A-4601-93AB-80CFDC2604F7}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{9877AA6D-D838-4FAC-BF31-FB1E9FB6CF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2DB82B6-1712-4481-9482-275C638BB411}"/>
   <bookViews>
     <workbookView xWindow="924" yWindow="2388" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,7 +82,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t xml:space="preserve">{StartDate} - {EndDate} </t>
+      <t xml:space="preserve">{StartDate} - {EndDate:dd.MM} </t>
     </r>
     <r>
       <rPr>
@@ -1963,7 +1963,7 @@
   <dimension ref="A1:E298"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="9.6"/>
@@ -4103,6 +4103,53 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B297:E297"/>
+    <mergeCell ref="B290:E290"/>
+    <mergeCell ref="B283:E283"/>
+    <mergeCell ref="B257:E257"/>
+    <mergeCell ref="B261:E261"/>
+    <mergeCell ref="B253:E253"/>
+    <mergeCell ref="B245:E245"/>
+    <mergeCell ref="B249:E249"/>
+    <mergeCell ref="B241:E241"/>
+    <mergeCell ref="B237:E237"/>
+    <mergeCell ref="B227:E227"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="B215:E215"/>
+    <mergeCell ref="B219:E219"/>
+    <mergeCell ref="B211:E211"/>
+    <mergeCell ref="B203:E203"/>
+    <mergeCell ref="B207:E207"/>
+    <mergeCell ref="B199:E199"/>
+    <mergeCell ref="B192:E192"/>
+    <mergeCell ref="B188:E188"/>
+    <mergeCell ref="B181:E181"/>
+    <mergeCell ref="B174:E174"/>
+    <mergeCell ref="B161:E161"/>
+    <mergeCell ref="B157:E157"/>
+    <mergeCell ref="B149:E149"/>
+    <mergeCell ref="B153:E153"/>
+    <mergeCell ref="B145:E145"/>
+    <mergeCell ref="B137:E137"/>
+    <mergeCell ref="B141:E141"/>
+    <mergeCell ref="B133:E133"/>
+    <mergeCell ref="B126:E126"/>
+    <mergeCell ref="B118:E118"/>
+    <mergeCell ref="B122:E122"/>
+    <mergeCell ref="B114:E114"/>
+    <mergeCell ref="B107:E107"/>
+    <mergeCell ref="B103:E103"/>
+    <mergeCell ref="B99:E99"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B39:E39"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B21:E21"/>
@@ -4110,53 +4157,6 @@
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A3:E3"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B99:E99"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="B118:E118"/>
-    <mergeCell ref="B122:E122"/>
-    <mergeCell ref="B114:E114"/>
-    <mergeCell ref="B107:E107"/>
-    <mergeCell ref="B103:E103"/>
-    <mergeCell ref="B145:E145"/>
-    <mergeCell ref="B137:E137"/>
-    <mergeCell ref="B141:E141"/>
-    <mergeCell ref="B133:E133"/>
-    <mergeCell ref="B126:E126"/>
-    <mergeCell ref="B181:E181"/>
-    <mergeCell ref="B174:E174"/>
-    <mergeCell ref="B161:E161"/>
-    <mergeCell ref="B157:E157"/>
-    <mergeCell ref="B149:E149"/>
-    <mergeCell ref="B153:E153"/>
-    <mergeCell ref="B203:E203"/>
-    <mergeCell ref="B207:E207"/>
-    <mergeCell ref="B199:E199"/>
-    <mergeCell ref="B192:E192"/>
-    <mergeCell ref="B188:E188"/>
-    <mergeCell ref="B227:E227"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="B215:E215"/>
-    <mergeCell ref="B219:E219"/>
-    <mergeCell ref="B211:E211"/>
-    <mergeCell ref="B253:E253"/>
-    <mergeCell ref="B245:E245"/>
-    <mergeCell ref="B249:E249"/>
-    <mergeCell ref="B241:E241"/>
-    <mergeCell ref="B237:E237"/>
-    <mergeCell ref="B297:E297"/>
-    <mergeCell ref="B290:E290"/>
-    <mergeCell ref="B283:E283"/>
-    <mergeCell ref="B257:E257"/>
-    <mergeCell ref="B261:E261"/>
   </mergeCells>
   <pageMargins left="0.19685" right="0" top="0.19685" bottom="0.49212600000000001" header="0.19685" footer="0.19685"/>
   <pageSetup orientation="landscape"/>

</xml_diff>